<commit_message>
go back to beta build
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="335">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -169,30 +169,6 @@
     <t xml:space="preserve">Event name (translated if using default event names)</t>
   </si>
   <si>
-    <t xml:space="preserve">\\q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event type 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event type 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event type 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event type 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">\\0</t>
   </si>
   <si>
@@ -265,42 +241,6 @@
     <t xml:space="preserve">OPEN (translated, respecting button state)</t>
   </si>
   <si>
-    <t xml:space="preserve">\\a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTO (translated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANUAL (translated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUTO (translated, respecting button state)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANUAL (translated, respecting button state)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HEATING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\\l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COOLING</t>
-  </si>
-  <si>
     <t xml:space="preserve">COMMANDS</t>
   </si>
   <si>
@@ -863,12 +803,6 @@
   </si>
   <si>
     <t xml:space="preserve">sets the PID target set value SV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pidSVC(&lt;int&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sets the PID target set value SV given in C</t>
   </si>
   <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
@@ -1224,10 +1158,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1327,10 +1261,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="1" sqref="B45:C45 B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
@@ -1445,13 +1379,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B45:C45 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1581,86 +1515,6 @@
       </c>
       <c r="B17" s="0" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1679,13 +1533,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B45" activeCellId="0" sqref="B45:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1694,32 +1548,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1581,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>3</v>
@@ -1735,1193 +1589,1185 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="3" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="3" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="3" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="3" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="3" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="3" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="3" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="3" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="3" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="3" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="3" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="3" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="3" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="3" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="3" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="3" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="3" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="3" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="3" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="3" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="3" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="3" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="3" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="3" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="3" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="3" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="3" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="3" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="3" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="3" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="3" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="3" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="3" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="3" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="3" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="3" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="3" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="3" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="3" t="s">
-        <v>272</v>
+        <v>252</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>273</v>
+        <v>253</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="3" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="3" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="3" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="3" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="3" t="s">
-        <v>282</v>
+        <v>262</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>283</v>
+        <v>263</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="3" t="s">
-        <v>284</v>
+        <v>264</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="3" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="3" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="3" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="3" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="3" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="3" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>278</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="3" t="s">
-        <v>300</v>
+        <v>98</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>301</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="3" t="s">
-        <v>118</v>
+        <v>280</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>119</v>
+        <v>281</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="3" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="3" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="3" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="3" t="s">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="3" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="3" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="3" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="3" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="3" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="3" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="3" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="3" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>306</v>
+      </c>
       <c r="B132" s="3" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>328</v>
-      </c>
       <c r="B133" s="3" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="3" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B135" s="3" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="3" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="3" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="3" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="3" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="3" t="s">
-        <v>343</v>
+        <v>197</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="3" t="s">
-        <v>217</v>
+        <v>324</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="3" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="3" t="s">
-        <v>348</v>
+        <v>206</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>329</v>
+      </c>
       <c r="B144" s="3" t="s">
-        <v>226</v>
+        <v>90</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>350</v>
+        <v>91</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>351</v>
-      </c>
       <c r="B145" s="3" t="s">
-        <v>110</v>
+        <v>330</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="3" t="s">
-        <v>352</v>
+        <v>92</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>353</v>
+        <v>93</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B147" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C147" s="0" t="s">
-        <v>113</v>
+        <v>94</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="3" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>354</v>
+        <v>99</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="3" t="s">
-        <v>118</v>
+        <v>333</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="C151" s="0" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restore dependency files based on b9103d0
see ultra minor changes f70e01f (921) on this repository
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Options" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Labels" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Commands" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,11 +23,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="357">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
   <si>
+    <t xml:space="preserve">tn:Button numbers can be drag and dropped to a new position. While holding the ALT key (Windows) / OPTION (macOS) buttons are swapped\n</t>
+  </si>
+  <si>
     <t xml:space="preserve">Column</t>
   </si>
   <si>
@@ -99,6 +103,18 @@
     <t xml:space="preserve">Applies one of 99 autogenerated color patterns to the buttons.  Set to "0" to manually choose the button colors.</t>
   </si>
   <si>
+    <t xml:space="preserve">Mark Last Pressed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invert state and color of last button pressed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooltips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show button specification as tooltips on hoovering a button</t>
+  </si>
+  <si>
     <t xml:space="preserve">Add</t>
   </si>
   <si>
@@ -129,6 +145,162 @@
     <t xml:space="preserve">Opens this window.</t>
   </si>
   <si>
+    <t xml:space="preserve">LABELS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn:The following substitutions are applied to button labels\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New line character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event name (translated if using default event names)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event type 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFF (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFF (translated, resepecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSE (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSE (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPEN (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTO (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL (translated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUTO (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUAL (translated, respecting button state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COOLING</t>
+  </si>
+  <si>
     <t xml:space="preserve">COMMANDS</t>
   </si>
   <si>
@@ -183,18 +355,36 @@
     <t xml:space="preserve">variable holding the last value read via MODBUS</t>
   </si>
   <si>
+    <t xml:space="preserve">$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable holding the last state of the button pressed (1 or 0)</t>
+  </si>
+  <si>
     <t xml:space="preserve">sleep(&lt;float&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sleep: add a delay of &lt;float&gt; seconds</t>
   </si>
   <si>
+    <t xml:space="preserve">button(i,b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button i to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
     <t xml:space="preserve">button(&lt;bool&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sets calling button to “pressed” if argument is 1 or True</t>
   </si>
   <si>
+    <t xml:space="preserve">button()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggles the state of the button</t>
+  </si>
+  <si>
     <t xml:space="preserve">read(slaveID,register)</t>
   </si>
   <si>
@@ -300,6 +490,9 @@
     <t xml:space="preserve">IO Command</t>
   </si>
   <si>
+    <t xml:space="preserve">variable holding the last result value</t>
+  </si>
+  <si>
     <t xml:space="preserve">set(c,b[,sn])</t>
   </si>
   <si>
@@ -354,6 +547,12 @@
     <t xml:space="preserve">YOCTOPUCE Relay Output: turn channel c of the relay module off</t>
   </si>
   <si>
+    <t xml:space="preserve">yset(c,b[,sn])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOCTOPUCE Relay Output: switches channel c of the relay module off (b=0) and on (b=1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">flip(c[,sn])</t>
   </si>
   <si>
@@ -381,7 +580,13 @@
     <t xml:space="preserve">button(i,c,b[,sn])</t>
   </si>
   <si>
-    <t xml:space="preserve">switches channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+    <t xml:space="preserve">switches PHIDGET Binary Output channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
   </si>
   <si>
     <t xml:space="preserve">santoker(&lt;target&gt;,&lt;value&gt;)</t>
@@ -390,6 +595,12 @@
     <t xml:space="preserve">sends integer &lt;value&gt; to &lt;target&gt; register specified by as byte in hex notation like “fa” via the Santoker Network protocol</t>
   </si>
   <si>
+    <t xml:space="preserve">kaleido(&lt;target&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends &lt;value&gt; to &lt;target&gt; via the Kaleido Serial or Network protocol</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hottop Heater</t>
   </si>
   <si>
@@ -654,6 +865,12 @@
     <t xml:space="preserve">sets the PID target set value SV</t>
   </si>
   <si>
+    <t xml:space="preserve">pidSVC(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the PID target set value SV given in C</t>
+  </si>
+  <si>
     <t xml:space="preserve">pidRS(&lt;rs&gt;)</t>
   </si>
   <si>
@@ -708,10 +925,10 @@
     <t xml:space="preserve">resets canvas color</t>
   </si>
   <si>
-    <t xml:space="preserve">button(&lt;name&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } </t>
+    <t xml:space="preserve">button(&lt;name&gt;|&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } ; sets calling button to “pressed” if argument is 1 or True</t>
   </si>
   <si>
     <t xml:space="preserve">palette(&lt;p&gt;)</t>
@@ -966,8 +1183,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1000,15 +1221,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
   </cols>
   <sheetData>
@@ -1017,70 +1238,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
+      <c r="B10" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1097,93 +1324,109 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
+      <c r="A8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
+      <c r="A9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
+      <c r="A10" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1202,1089 +1445,1483 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C151"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C107" activeCellId="0" sqref="C107"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="102.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>107</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
-        <v>53</v>
+      <c r="B12" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
-        <v>55</v>
+      <c r="B13" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>58</v>
+      <c r="B14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
-        <v>59</v>
+      <c r="B15" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
-        <v>61</v>
+      <c r="B16" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
-        <v>63</v>
+      <c r="B17" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
-        <v>65</v>
+      <c r="B18" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
-        <v>67</v>
+      <c r="B19" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
-        <v>69</v>
+      <c r="B20" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
-        <v>71</v>
+      <c r="B21" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2" t="s">
-        <v>73</v>
+      <c r="B22" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
-        <v>75</v>
+      <c r="B23" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2" t="s">
-        <v>77</v>
+      <c r="B24" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="s">
-        <v>79</v>
+      <c r="B25" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2" t="s">
-        <v>81</v>
+      <c r="B26" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2" t="s">
-        <v>83</v>
+      <c r="B27" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="2" t="s">
-        <v>85</v>
+      <c r="B28" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2" t="s">
-        <v>87</v>
+      <c r="B29" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>90</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>92</v>
+      <c r="B31" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2" t="s">
-        <v>94</v>
+      <c r="B32" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>97</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2" t="s">
-        <v>98</v>
+      <c r="A34" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2" t="s">
-        <v>100</v>
+      <c r="B35" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2" t="s">
-        <v>102</v>
+      <c r="B36" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>103</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="2" t="s">
-        <v>104</v>
+      <c r="B37" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2" t="s">
-        <v>106</v>
+      <c r="B38" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>107</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
-        <v>108</v>
+      <c r="B39" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
-        <v>110</v>
+      <c r="B40" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C54" s="0" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="2" t="s">
-        <v>141</v>
+      <c r="B55" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>142</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="2" t="s">
-        <v>143</v>
+      <c r="B56" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2" t="s">
-        <v>145</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>192</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="2" t="s">
-        <v>147</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>194</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="2" t="s">
-        <v>149</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>150</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="2" t="s">
-        <v>151</v>
+      <c r="A60" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>154</v>
+      <c r="A61" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>156</v>
+        <v>204</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="2" t="s">
-        <v>158</v>
+      <c r="B63" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="2" t="s">
-        <v>160</v>
+      <c r="B64" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="2" t="s">
-        <v>162</v>
+      <c r="B65" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="2" t="s">
-        <v>53</v>
+      <c r="B66" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>54</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>51</v>
+      <c r="B67" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="2" t="s">
-        <v>53</v>
+      <c r="B68" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>54</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="2" t="s">
-        <v>55</v>
+      <c r="B69" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="2" t="s">
-        <v>166</v>
+      <c r="B70" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>167</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="2" t="s">
-        <v>168</v>
+      <c r="B71" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>169</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="2" t="s">
-        <v>170</v>
+      <c r="A72" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="2" t="s">
-        <v>172</v>
+      <c r="B73" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>173</v>
+        <v>229</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="2" t="s">
-        <v>174</v>
+      <c r="B74" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>175</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="2" t="s">
-        <v>176</v>
+      <c r="B75" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>177</v>
+        <v>233</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="2" t="s">
-        <v>178</v>
+      <c r="B76" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>180</v>
+        <v>234</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>181</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>182</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>186</v>
+      <c r="B80" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>188</v>
+      <c r="B81" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="2" t="s">
-        <v>190</v>
+      <c r="B82" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2" t="s">
-        <v>192</v>
+      <c r="B83" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="C83" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C85" s="0" t="s">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="2" t="s">
-        <v>208</v>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>252</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>209</v>
+        <v>253</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="2" t="s">
-        <v>210</v>
+      <c r="A93" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="2" t="s">
-        <v>212</v>
+      <c r="A94" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="2" t="s">
-        <v>214</v>
+      <c r="B95" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="2" t="s">
-        <v>216</v>
+      <c r="B96" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="C96" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B136" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B137" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C97" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="2" t="s">
+      <c r="C141" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C101" s="0" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C104" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C106" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C114" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C115" s="0" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C120" s="0" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C121" s="0" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C127" s="0" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C129" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C130" s="0" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C131" s="0" t="s">
-        <v>284</v>
+      <c r="C144" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upto e3bfc1 plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -685,6 +685,36 @@
   </si>
   <si>
     <t xml:space="preserve">moves the background profile the indicated number of steps towards &lt;direction&gt;, with &lt;direction&gt; one of up, down, left, right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables keyboard mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -883,7 +913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -893,7 +923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -971,7 +1001,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -980,7 +1010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -990,7 +1020,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1076,7 +1106,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1085,21 +1115,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,50 +1931,50 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C99" s="0" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="0" t="s">
+      <c r="C100" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C100" s="0" t="s">
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
+      <c r="C101" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C101" s="0" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+      <c r="C102" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C102" s="0" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="C103" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
         <v>232</v>
       </c>
@@ -1970,75 +2000,115 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>128</v>
+        <v>238</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>137</v>
+        <v>244</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>244</v>
-      </c>
       <c r="B111" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>55</v>
+        <v>249</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
downto 4b8a4 plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="250">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -685,36 +685,6 @@
   </si>
   <si>
     <t xml:space="preserve">moves the background profile the indicated number of steps towards &lt;direction&gt;, with &lt;direction&gt; one of up, down, left, right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keyboard(&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enables/disables keyboard mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -913,7 +883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -923,7 +893,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1001,7 +971,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1010,7 +980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1020,7 +990,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1106,7 +1076,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1115,21 +1085,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,50 +1901,50 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>221</v>
+      </c>
       <c r="B99" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>231</v>
-      </c>
       <c r="B104" s="0" t="s">
         <v>232</v>
       </c>
@@ -2000,115 +1970,75 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C107" s="0" t="s">
         <v>238</v>
-      </c>
-      <c r="C107" s="0" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>240</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>242</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="B111" s="0" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="0" t="s">
         <v>246</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>248</v>
+        <v>54</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>249</v>
+        <v>55</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="C115" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
upto be0805 plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="252">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t xml:space="preserve">moves the background profile the indicated number of steps towards &lt;direction&gt;, with &lt;direction&gt; one of up, down, left, right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keyboard(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enables/disables keyboard mode</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -883,7 +889,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -893,7 +899,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -971,7 +977,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -980,7 +986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -990,7 +996,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1076,7 +1082,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1085,21 +1091,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1901,18 +1907,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="C99" s="0" t="s">
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="0" t="s">
         <v>224</v>
       </c>
@@ -1970,15 +1976,15 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="0" t="s">
-        <v>128</v>
+        <v>238</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>239</v>
+        <v>128</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>240</v>
@@ -1994,51 +2000,60 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C110" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="B111" s="0" t="s">
+      <c r="C111" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="C111" s="0" t="s">
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="0" t="s">
-        <v>53</v>
+        <v>247</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>54</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>247</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>248</v>
+        <v>55</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>249</v>
       </c>
     </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
upto 52ab59 plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -691,6 +691,30 @@
   </si>
   <si>
     <t xml:space="preserve">enables/disables keyboard mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -899,7 +923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -996,7 +1020,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1095,13 +1119,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1048576"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1915,42 +1939,42 @@
         <v>222</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B100" s="0" t="s">
+      <c r="C100" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C100" s="0" t="s">
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="0" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="0" t="s">
+      <c r="C101" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="C101" s="0" t="s">
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="0" t="s">
+      <c r="C102" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="C102" s="0" t="s">
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="0" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="0" t="s">
+      <c r="C103" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C103" s="0" t="s">
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="0" t="s">
         <v>232</v>
       </c>
@@ -1984,42 +2008,39 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
-        <v>246</v>
-      </c>
       <c r="B112" s="0" t="s">
-        <v>247</v>
+        <v>128</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>248</v>
@@ -2027,29 +2048,63 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>53</v>
+        <v>249</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>55</v>
+        <v>251</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>250</v>
+        <v>137</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
downto 4a1a5c plus build files
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="252">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -691,30 +691,6 @@
   </si>
   <si>
     <t xml:space="preserve">enables/disables keyboard mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showCurve(&lt;name&gt;,&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the curve indicated by &lt;name&gt; which is one of { ET, BT, DeltaET, DeltaBT, BackgroundET, BackgroundBT}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showExtraCurve(&lt;extra_device&gt;,&lt;curve&gt;,&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the &lt;curve&gt; (one of {T1,T2}) of the zero-based &lt;extra_device&gt; number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showEvents(&lt;event_type&gt;, &lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the events of &lt;event_type&gt; in [1,..,5]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showBackgroundEvents(&lt;bool&gt;)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows/hides the events of the background profile</t>
   </si>
   <si>
     <t xml:space="preserve">RC Command</t>
@@ -923,7 +899,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1020,7 +996,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.86"/>
@@ -1119,13 +1095,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="C101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.53"/>
@@ -1939,42 +1915,42 @@
         <v>222</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>223</v>
+      </c>
       <c r="B100" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>231</v>
-      </c>
       <c r="B104" s="0" t="s">
         <v>232</v>
       </c>
@@ -2008,39 +1984,42 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>240</v>
-      </c>
-      <c r="C108" s="0" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>242</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C110" s="0" t="s">
         <v>244</v>
-      </c>
-      <c r="C110" s="0" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C111" s="0" t="s">
+      <c r="B112" s="0" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="0" t="s">
-        <v>128</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>248</v>
@@ -2048,63 +2027,29 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>249</v>
+        <v>53</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>250</v>
+        <v>54</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="0" t="s">
-        <v>251</v>
+        <v>55</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="0" t="s">
-        <v>137</v>
+        <v>250</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C117" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
up to 37a392e, linux only
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="373">
   <si>
     <t xml:space="preserve">EVENT CUSTOM BUTTONS</t>
   </si>
@@ -319,13 +319,31 @@
     <t xml:space="preserve">COOLING</t>
   </si>
   <si>
+    <t xml:space="preserve">\\V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value interpreted as temperature in Fahrenheit converted to the current temperature mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">\\T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">event value interpreted as temperature in Celsius converted to the current temperature mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">COMMANDS</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by the current button value plus the offset for \u00B1 event types.  If a placeholder occurs several times in a description/command, all those occurrences are replaced by the value.\n</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value, and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: Commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -1280,10 +1298,10 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="32:32 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
@@ -1382,10 +1400,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="32:32 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
@@ -1500,13 +1518,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="32:32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1740,6 +1758,30 @@
       </c>
       <c r="B30" s="0" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1761,49 +1803,49 @@
   <dimension ref="A1:C153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="32:32 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="115.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="100.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1853,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>3</v>
@@ -1819,1201 +1861,1201 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="2" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="2" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="2" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="2" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="2" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="2" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="2" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="2" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="2" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="2" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="2" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="2" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="2" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="2" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="2" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="2" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B105" s="2" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="2" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B112" s="2" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="2" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="2" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="2" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="2" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="2" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="2" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B131" s="2" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B132" s="2" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B133" s="2" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="2" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="2" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B137" s="2" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B138" s="2" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B139" s="2" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B140" s="2" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B141" s="2" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B142" s="2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B143" s="2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="2" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="2" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B146" s="2" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B148" s="2" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B149" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B150" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B151" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B152" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B153" s="2" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up to 1c4e351, win only
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventbuttons.xlsx
+++ b/doc/help_dialogs/Input_files/eventbuttons.xlsx
@@ -517,7 +517,7 @@
     <t xml:space="preserve">write(slaveId,register,value) or write([slaveId,register,value],..,[slaveId,register,value])</t>
   </si>
   <si>
-    <t xml:space="preserve">write register: MODBUS function 6 (int) or function 16 (float)</t>
+    <t xml:space="preserve">deprecated: use writeSingle for MODBUS function 6 (int) or writeWord for function 16 (float)</t>
   </si>
   <si>
     <t xml:space="preserve">wcoil(slaveId,register,&lt;bool&gt;)</t>
@@ -1593,7 +1593,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="126:126 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="126:126 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="126:126 A28"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2121,15 +2121,15 @@
   </sheetPr>
   <dimension ref="A1:C163"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A117" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A126" activeCellId="0" sqref="126:126"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="58.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="69.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.82"/>
   </cols>
   <sheetData>

</xml_diff>